<commit_message>
Last commit (I hope)
</commit_message>
<xml_diff>
--- a/Wyniki.xlsx
+++ b/Wyniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mateuszmuziol/Documents/PEA/PEA Projekt 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0546EF-BE07-FF4C-8CED-6228C813A7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2052560A-EB6E-8A48-8BBC-574A189F7CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,9 +335,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,6 +379,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,11 +482,9 @@
             <c:v>Brute Force</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -508,6 +506,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="40134"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Wyniki uśrednione + tabelki'!$C$2:$I$2</c:f>
@@ -576,11 +624,9 @@
             <c:v>Branch &amp; Bound</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -602,6 +648,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Wyniki uśrednione + tabelki'!$C$2:$I$2</c:f>
@@ -1106,11 +1196,9 @@
             <c:v>Przegląd zupełny</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1132,6 +1220,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Wyniki uśrednione + tabelki'!$C$2:$G$2</c:f>
@@ -1672,12 +1804,11 @@
             <c:v>Branch &amp; Bound</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="9525" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:alpha val="50000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="solid"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1698,6 +1829,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="pl-PL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Wyniki uśrednione + tabelki'!$C$2:$I$2</c:f>
@@ -4330,41 +4505,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>6</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="F2" s="9">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="F2" s="8">
         <v>8</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="J2" s="9">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="J2" s="8">
         <v>9</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="N2" s="9">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="N2" s="8">
         <v>10</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="R2" s="9">
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="R2" s="8">
         <v>12</v>
       </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="V2" s="9">
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="V2" s="8">
         <v>13</v>
       </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Z2" s="9">
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Z2" s="8">
         <v>14</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -4477,7 +4652,7 @@
       <c r="T4" s="2">
         <v>2283</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="W4" s="2">
@@ -4486,7 +4661,7 @@
       <c r="X4" s="2">
         <v>3235</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" s="9" t="s">
         <v>5</v>
       </c>
       <c r="AA4" s="2">
@@ -4542,14 +4717,14 @@
       <c r="T5" s="2">
         <v>2259</v>
       </c>
-      <c r="V5" s="10"/>
+      <c r="V5" s="9"/>
       <c r="W5" s="2">
         <v>16445</v>
       </c>
       <c r="X5" s="2">
         <v>3008</v>
       </c>
-      <c r="Z5" s="10"/>
+      <c r="Z5" s="9"/>
       <c r="AA5" s="2">
         <v>3932</v>
       </c>
@@ -4603,14 +4778,14 @@
       <c r="T6" s="2">
         <v>2253</v>
       </c>
-      <c r="V6" s="10"/>
+      <c r="V6" s="9"/>
       <c r="W6" s="2">
         <v>16030</v>
       </c>
       <c r="X6" s="2">
         <v>3004</v>
       </c>
-      <c r="Z6" s="10"/>
+      <c r="Z6" s="9"/>
       <c r="AA6" s="2">
         <v>4038</v>
       </c>
@@ -4664,14 +4839,14 @@
       <c r="T7" s="2">
         <v>2249</v>
       </c>
-      <c r="V7" s="10"/>
+      <c r="V7" s="9"/>
       <c r="W7" s="2">
         <v>16604</v>
       </c>
       <c r="X7" s="2">
         <v>3016</v>
       </c>
-      <c r="Z7" s="10"/>
+      <c r="Z7" s="9"/>
       <c r="AA7" s="2">
         <v>4043</v>
       </c>
@@ -4725,14 +4900,14 @@
       <c r="T8" s="2">
         <v>1967</v>
       </c>
-      <c r="V8" s="10"/>
+      <c r="V8" s="9"/>
       <c r="W8" s="2">
         <v>16080</v>
       </c>
       <c r="X8" s="2">
         <v>3001</v>
       </c>
-      <c r="Z8" s="10"/>
+      <c r="Z8" s="9"/>
       <c r="AA8" s="2">
         <v>4020</v>
       </c>
@@ -4786,14 +4961,14 @@
       <c r="T9" s="2">
         <v>2255</v>
       </c>
-      <c r="V9" s="10"/>
+      <c r="V9" s="9"/>
       <c r="W9" s="2">
         <v>16591</v>
       </c>
       <c r="X9" s="2">
         <v>3005</v>
       </c>
-      <c r="Z9" s="10"/>
+      <c r="Z9" s="9"/>
       <c r="AA9" s="2">
         <v>4012</v>
       </c>
@@ -4847,14 +5022,14 @@
       <c r="T10" s="2">
         <v>2188</v>
       </c>
-      <c r="V10" s="10"/>
+      <c r="V10" s="9"/>
       <c r="W10" s="2">
         <v>16141</v>
       </c>
       <c r="X10" s="2">
         <v>3007</v>
       </c>
-      <c r="Z10" s="10"/>
+      <c r="Z10" s="9"/>
       <c r="AA10" s="2">
         <v>4246</v>
       </c>
@@ -4908,14 +5083,14 @@
       <c r="T11" s="2">
         <v>2153</v>
       </c>
-      <c r="V11" s="10"/>
+      <c r="V11" s="9"/>
       <c r="W11" s="2">
         <v>16704</v>
       </c>
       <c r="X11" s="2">
         <v>3019</v>
       </c>
-      <c r="Z11" s="10"/>
+      <c r="Z11" s="9"/>
       <c r="AA11" s="2">
         <v>4486</v>
       </c>
@@ -4969,14 +5144,14 @@
       <c r="T12" s="2">
         <v>2233</v>
       </c>
-      <c r="V12" s="10"/>
+      <c r="V12" s="9"/>
       <c r="W12" s="2">
         <v>16091</v>
       </c>
       <c r="X12" s="2">
         <v>3002</v>
       </c>
-      <c r="Z12" s="10"/>
+      <c r="Z12" s="9"/>
       <c r="AA12" s="2">
         <v>4089</v>
       </c>
@@ -5030,14 +5205,14 @@
       <c r="T13" s="2">
         <v>2248</v>
       </c>
-      <c r="V13" s="10"/>
+      <c r="V13" s="9"/>
       <c r="W13" s="2">
         <v>16657</v>
       </c>
       <c r="X13" s="2">
         <v>3001</v>
       </c>
-      <c r="Z13" s="10"/>
+      <c r="Z13" s="9"/>
       <c r="AA13" s="2">
         <v>4065</v>
       </c>
@@ -5091,14 +5266,14 @@
       <c r="T14" s="2">
         <v>2235</v>
       </c>
-      <c r="V14" s="10"/>
+      <c r="V14" s="9"/>
       <c r="W14" s="2">
         <v>16109</v>
       </c>
       <c r="X14" s="2">
         <v>3008</v>
       </c>
-      <c r="Z14" s="10"/>
+      <c r="Z14" s="9"/>
       <c r="AA14" s="2">
         <v>4049</v>
       </c>
@@ -5152,14 +5327,14 @@
       <c r="T15" s="2">
         <v>2233</v>
       </c>
-      <c r="V15" s="10"/>
+      <c r="V15" s="9"/>
       <c r="W15" s="2">
         <v>16644</v>
       </c>
       <c r="X15" s="2">
         <v>3026</v>
       </c>
-      <c r="Z15" s="10"/>
+      <c r="Z15" s="9"/>
       <c r="AA15" s="2">
         <v>4034</v>
       </c>
@@ -5213,14 +5388,14 @@
       <c r="T16" s="2">
         <v>2235</v>
       </c>
-      <c r="V16" s="10"/>
+      <c r="V16" s="9"/>
       <c r="W16" s="2">
         <v>16336</v>
       </c>
       <c r="X16" s="2">
         <v>3015</v>
       </c>
-      <c r="Z16" s="10"/>
+      <c r="Z16" s="9"/>
       <c r="AA16" s="2">
         <v>4039</v>
       </c>
@@ -5274,14 +5449,14 @@
       <c r="T17" s="2">
         <v>1935</v>
       </c>
-      <c r="V17" s="10"/>
+      <c r="V17" s="9"/>
       <c r="W17" s="2">
         <v>16506</v>
       </c>
       <c r="X17" s="2">
         <v>3011</v>
       </c>
-      <c r="Z17" s="10"/>
+      <c r="Z17" s="9"/>
       <c r="AA17" s="2">
         <v>4065</v>
       </c>
@@ -5335,14 +5510,14 @@
       <c r="T18" s="2">
         <v>1923</v>
       </c>
-      <c r="V18" s="10"/>
+      <c r="V18" s="9"/>
       <c r="W18" s="2">
         <v>16582</v>
       </c>
       <c r="X18" s="2">
         <v>3012</v>
       </c>
-      <c r="Z18" s="10"/>
+      <c r="Z18" s="9"/>
       <c r="AA18" s="2">
         <v>4526</v>
       </c>
@@ -5396,14 +5571,14 @@
       <c r="T19" s="2">
         <v>2234</v>
       </c>
-      <c r="V19" s="10"/>
+      <c r="V19" s="9"/>
       <c r="W19" s="2">
         <v>16193</v>
       </c>
       <c r="X19" s="2">
         <v>3028</v>
       </c>
-      <c r="Z19" s="10"/>
+      <c r="Z19" s="9"/>
       <c r="AA19" s="2">
         <v>4088</v>
       </c>
@@ -5457,14 +5632,14 @@
       <c r="T20" s="2">
         <v>2230</v>
       </c>
-      <c r="V20" s="10"/>
+      <c r="V20" s="9"/>
       <c r="W20" s="2">
         <v>1171</v>
       </c>
       <c r="X20" s="2">
         <v>3041</v>
       </c>
-      <c r="Z20" s="10"/>
+      <c r="Z20" s="9"/>
       <c r="AA20" s="2">
         <v>4050</v>
       </c>
@@ -5518,14 +5693,14 @@
       <c r="T21" s="2">
         <v>1328</v>
       </c>
-      <c r="V21" s="10"/>
+      <c r="V21" s="9"/>
       <c r="W21" s="2">
         <v>1166</v>
       </c>
       <c r="X21" s="2">
         <v>3032</v>
       </c>
-      <c r="Z21" s="10"/>
+      <c r="Z21" s="9"/>
       <c r="AA21" s="2">
         <v>4076</v>
       </c>
@@ -5579,14 +5754,14 @@
       <c r="T22" s="2">
         <v>1331</v>
       </c>
-      <c r="V22" s="10"/>
+      <c r="V22" s="9"/>
       <c r="W22" s="2">
         <v>1168</v>
       </c>
       <c r="X22" s="2">
         <v>3022</v>
       </c>
-      <c r="Z22" s="10"/>
+      <c r="Z22" s="9"/>
       <c r="AA22" s="2">
         <v>4040</v>
       </c>
@@ -5640,14 +5815,14 @@
       <c r="T23" s="2">
         <v>1326</v>
       </c>
-      <c r="V23" s="10"/>
+      <c r="V23" s="9"/>
       <c r="W23" s="2">
         <v>1154</v>
       </c>
       <c r="X23" s="2">
         <v>3038</v>
       </c>
-      <c r="Z23" s="10"/>
+      <c r="Z23" s="9"/>
       <c r="AA23" s="2">
         <v>4048</v>
       </c>
@@ -5701,14 +5876,14 @@
       <c r="T24" s="2">
         <v>1323</v>
       </c>
-      <c r="V24" s="10"/>
+      <c r="V24" s="9"/>
       <c r="W24" s="2">
         <v>1155</v>
       </c>
       <c r="X24" s="2">
         <v>3026</v>
       </c>
-      <c r="Z24" s="10"/>
+      <c r="Z24" s="9"/>
       <c r="AA24" s="2">
         <v>4054</v>
       </c>
@@ -5762,14 +5937,14 @@
       <c r="T25" s="2">
         <v>1332</v>
       </c>
-      <c r="V25" s="10"/>
+      <c r="V25" s="9"/>
       <c r="W25" s="2">
         <v>1159</v>
       </c>
       <c r="X25" s="2">
         <v>3033</v>
       </c>
-      <c r="Z25" s="10"/>
+      <c r="Z25" s="9"/>
       <c r="AA25" s="2">
         <v>4269</v>
       </c>
@@ -5823,14 +5998,14 @@
       <c r="T26" s="2">
         <v>1328</v>
       </c>
-      <c r="V26" s="10"/>
+      <c r="V26" s="9"/>
       <c r="W26" s="2">
         <v>1173</v>
       </c>
       <c r="X26" s="2">
         <v>3036</v>
       </c>
-      <c r="Z26" s="10"/>
+      <c r="Z26" s="9"/>
       <c r="AA26" s="2">
         <v>4523</v>
       </c>
@@ -5884,14 +6059,14 @@
       <c r="T27" s="2">
         <v>1334</v>
       </c>
-      <c r="V27" s="10"/>
+      <c r="V27" s="9"/>
       <c r="W27" s="2">
         <v>1174</v>
       </c>
       <c r="X27" s="2">
         <v>3028</v>
       </c>
-      <c r="Z27" s="10"/>
+      <c r="Z27" s="9"/>
       <c r="AA27" s="2">
         <v>4123</v>
       </c>
@@ -5945,14 +6120,14 @@
       <c r="T28" s="2">
         <v>1336</v>
       </c>
-      <c r="V28" s="10"/>
+      <c r="V28" s="9"/>
       <c r="W28" s="2">
         <v>1223</v>
       </c>
       <c r="X28" s="2">
         <v>3036</v>
       </c>
-      <c r="Z28" s="10"/>
+      <c r="Z28" s="9"/>
       <c r="AA28" s="2">
         <v>4082</v>
       </c>
@@ -6006,14 +6181,14 @@
       <c r="T29" s="2">
         <v>1326</v>
       </c>
-      <c r="V29" s="10"/>
+      <c r="V29" s="9"/>
       <c r="W29" s="3">
         <v>1265</v>
       </c>
       <c r="X29" s="2">
         <v>3029</v>
       </c>
-      <c r="Z29" s="10"/>
+      <c r="Z29" s="9"/>
       <c r="AA29" s="2">
         <v>4057</v>
       </c>
@@ -6067,14 +6242,14 @@
       <c r="T30" s="2">
         <v>1327</v>
       </c>
-      <c r="V30" s="10"/>
+      <c r="V30" s="9"/>
       <c r="W30" s="2">
         <v>1268</v>
       </c>
       <c r="X30" s="2">
         <v>3028</v>
       </c>
-      <c r="Z30" s="10"/>
+      <c r="Z30" s="9"/>
       <c r="AA30" s="2">
         <v>4077</v>
       </c>
@@ -6128,14 +6303,14 @@
       <c r="T31" s="2">
         <v>1331</v>
       </c>
-      <c r="V31" s="10"/>
+      <c r="V31" s="9"/>
       <c r="W31" s="2">
         <v>1316</v>
       </c>
       <c r="X31" s="2">
         <v>3039</v>
       </c>
-      <c r="Z31" s="10"/>
+      <c r="Z31" s="9"/>
       <c r="AA31" s="2">
         <v>4074</v>
       </c>
@@ -6189,14 +6364,14 @@
       <c r="T32" s="2">
         <v>1334</v>
       </c>
-      <c r="V32" s="10"/>
+      <c r="V32" s="9"/>
       <c r="W32" s="2">
         <v>1329</v>
       </c>
       <c r="X32" s="2">
         <v>3041</v>
       </c>
-      <c r="Z32" s="10"/>
+      <c r="Z32" s="9"/>
       <c r="AA32" s="2">
         <v>4099</v>
       </c>
@@ -6250,14 +6425,14 @@
       <c r="T33" s="2">
         <v>1337</v>
       </c>
-      <c r="V33" s="10"/>
+      <c r="V33" s="9"/>
       <c r="W33" s="2">
         <v>1200</v>
       </c>
       <c r="X33" s="2">
         <v>3025</v>
       </c>
-      <c r="Z33" s="10"/>
+      <c r="Z33" s="9"/>
       <c r="AA33" s="2">
         <v>4536</v>
       </c>
@@ -6311,14 +6486,14 @@
       <c r="T34" s="2">
         <v>1335</v>
       </c>
-      <c r="V34" s="10"/>
+      <c r="V34" s="9"/>
       <c r="W34" s="2">
         <v>1183</v>
       </c>
       <c r="X34" s="2">
         <v>3053</v>
       </c>
-      <c r="Z34" s="10"/>
+      <c r="Z34" s="9"/>
       <c r="AA34" s="2">
         <v>4102</v>
       </c>
@@ -6372,14 +6547,14 @@
       <c r="T35" s="2">
         <v>1333</v>
       </c>
-      <c r="V35" s="10"/>
+      <c r="V35" s="9"/>
       <c r="W35" s="2">
         <v>1177</v>
       </c>
       <c r="X35" s="2">
         <v>3049</v>
       </c>
-      <c r="Z35" s="10"/>
+      <c r="Z35" s="9"/>
       <c r="AA35" s="2">
         <v>4068</v>
       </c>
@@ -6433,14 +6608,14 @@
       <c r="T36" s="2">
         <v>1338</v>
       </c>
-      <c r="V36" s="10"/>
+      <c r="V36" s="9"/>
       <c r="W36" s="2">
         <v>1171</v>
       </c>
       <c r="X36" s="2">
         <v>3045</v>
       </c>
-      <c r="Z36" s="10"/>
+      <c r="Z36" s="9"/>
       <c r="AA36" s="2">
         <v>4067</v>
       </c>
@@ -6494,14 +6669,14 @@
       <c r="T37" s="2">
         <v>1338</v>
       </c>
-      <c r="V37" s="10"/>
+      <c r="V37" s="9"/>
       <c r="W37" s="2">
         <v>1172</v>
       </c>
       <c r="X37" s="2">
         <v>3034</v>
       </c>
-      <c r="Z37" s="10"/>
+      <c r="Z37" s="9"/>
       <c r="AA37" s="2">
         <v>4066</v>
       </c>
@@ -6555,14 +6730,14 @@
       <c r="T38" s="2">
         <v>1331</v>
       </c>
-      <c r="V38" s="10"/>
+      <c r="V38" s="9"/>
       <c r="W38" s="2">
         <v>1176</v>
       </c>
       <c r="X38" s="2">
         <v>3028</v>
       </c>
-      <c r="Z38" s="10"/>
+      <c r="Z38" s="9"/>
       <c r="AA38" s="2">
         <v>4051</v>
       </c>
@@ -6616,14 +6791,14 @@
       <c r="T39" s="2">
         <v>1349</v>
       </c>
-      <c r="V39" s="10"/>
+      <c r="V39" s="9"/>
       <c r="W39" s="2">
         <v>1176</v>
       </c>
       <c r="X39" s="2">
         <v>3034</v>
       </c>
-      <c r="Z39" s="10"/>
+      <c r="Z39" s="9"/>
       <c r="AA39" s="2">
         <v>4054</v>
       </c>
@@ -6677,14 +6852,14 @@
       <c r="T40" s="2">
         <v>1341</v>
       </c>
-      <c r="V40" s="10"/>
+      <c r="V40" s="9"/>
       <c r="W40" s="2">
         <v>1165</v>
       </c>
       <c r="X40" s="2">
         <v>3026</v>
       </c>
-      <c r="Z40" s="10"/>
+      <c r="Z40" s="9"/>
       <c r="AA40" s="2">
         <v>4268</v>
       </c>
@@ -6738,14 +6913,14 @@
       <c r="T41" s="2">
         <v>1338</v>
       </c>
-      <c r="V41" s="10"/>
+      <c r="V41" s="9"/>
       <c r="W41" s="2">
         <v>1174</v>
       </c>
       <c r="X41" s="2">
         <v>3043</v>
       </c>
-      <c r="Z41" s="10"/>
+      <c r="Z41" s="9"/>
       <c r="AA41" s="2">
         <v>4516</v>
       </c>
@@ -6799,14 +6974,14 @@
       <c r="T42" s="2">
         <v>1338</v>
       </c>
-      <c r="V42" s="10"/>
+      <c r="V42" s="9"/>
       <c r="W42" s="2">
         <v>1169</v>
       </c>
       <c r="X42" s="2">
         <v>3038</v>
       </c>
-      <c r="Z42" s="10"/>
+      <c r="Z42" s="9"/>
       <c r="AA42" s="2">
         <v>4108</v>
       </c>
@@ -6860,14 +7035,14 @@
       <c r="T43" s="2">
         <v>1333</v>
       </c>
-      <c r="V43" s="10"/>
+      <c r="V43" s="9"/>
       <c r="W43" s="2">
         <v>1186</v>
       </c>
       <c r="X43" s="2">
         <v>3046</v>
       </c>
-      <c r="Z43" s="10"/>
+      <c r="Z43" s="9"/>
       <c r="AA43" s="2">
         <v>4071</v>
       </c>
@@ -6921,14 +7096,14 @@
       <c r="T44" s="2">
         <v>1335</v>
       </c>
-      <c r="V44" s="10"/>
+      <c r="V44" s="9"/>
       <c r="W44" s="2">
         <v>1168</v>
       </c>
       <c r="X44" s="2">
         <v>3041</v>
       </c>
-      <c r="Z44" s="10"/>
+      <c r="Z44" s="9"/>
       <c r="AA44" s="2">
         <v>4056</v>
       </c>
@@ -6982,14 +7157,14 @@
       <c r="T45" s="2">
         <v>1332</v>
       </c>
-      <c r="V45" s="10"/>
+      <c r="V45" s="9"/>
       <c r="W45" s="2">
         <v>1165</v>
       </c>
       <c r="X45" s="2">
         <v>3032</v>
       </c>
-      <c r="Z45" s="10"/>
+      <c r="Z45" s="9"/>
       <c r="AA45" s="2">
         <v>4063</v>
       </c>
@@ -7043,14 +7218,14 @@
       <c r="T46" s="2">
         <v>1337</v>
       </c>
-      <c r="V46" s="10"/>
+      <c r="V46" s="9"/>
       <c r="W46" s="2">
         <v>1163</v>
       </c>
       <c r="X46" s="2">
         <v>3041</v>
       </c>
-      <c r="Z46" s="10"/>
+      <c r="Z46" s="9"/>
       <c r="AA46" s="2">
         <v>4053</v>
       </c>
@@ -7104,14 +7279,14 @@
       <c r="T47" s="2">
         <v>1333</v>
       </c>
-      <c r="V47" s="10"/>
+      <c r="V47" s="9"/>
       <c r="W47" s="2">
         <v>1174</v>
       </c>
       <c r="X47" s="2">
         <v>3034</v>
       </c>
-      <c r="Z47" s="10"/>
+      <c r="Z47" s="9"/>
       <c r="AA47" s="2">
         <v>4072</v>
       </c>
@@ -7165,14 +7340,14 @@
       <c r="T48" s="2">
         <v>1334</v>
       </c>
-      <c r="V48" s="10"/>
+      <c r="V48" s="9"/>
       <c r="W48" s="2">
         <v>1184</v>
       </c>
       <c r="X48" s="2">
         <v>3026</v>
       </c>
-      <c r="Z48" s="10"/>
+      <c r="Z48" s="9"/>
       <c r="AA48" s="2">
         <v>4537</v>
       </c>
@@ -7226,14 +7401,14 @@
       <c r="T49" s="2">
         <v>1339</v>
       </c>
-      <c r="V49" s="10"/>
+      <c r="V49" s="9"/>
       <c r="W49" s="2">
         <v>1182</v>
       </c>
       <c r="X49" s="2">
         <v>3043</v>
       </c>
-      <c r="Z49" s="10"/>
+      <c r="Z49" s="9"/>
       <c r="AA49" s="2">
         <v>4137</v>
       </c>
@@ -7287,14 +7462,14 @@
       <c r="T50" s="2">
         <v>1330</v>
       </c>
-      <c r="V50" s="10"/>
+      <c r="V50" s="9"/>
       <c r="W50" s="2">
         <v>1174</v>
       </c>
       <c r="X50" s="2">
         <v>3041</v>
       </c>
-      <c r="Z50" s="10"/>
+      <c r="Z50" s="9"/>
       <c r="AA50" s="2">
         <v>4084</v>
       </c>
@@ -7348,14 +7523,14 @@
       <c r="T51" s="2">
         <v>1336</v>
       </c>
-      <c r="V51" s="10"/>
+      <c r="V51" s="9"/>
       <c r="W51" s="2">
         <v>1177</v>
       </c>
       <c r="X51" s="2">
         <v>3038</v>
       </c>
-      <c r="Z51" s="10"/>
+      <c r="Z51" s="9"/>
       <c r="AA51" s="2">
         <v>4085</v>
       </c>
@@ -7409,14 +7584,14 @@
       <c r="T52" s="2">
         <v>1338</v>
       </c>
-      <c r="V52" s="10"/>
+      <c r="V52" s="9"/>
       <c r="W52" s="2">
         <v>1171</v>
       </c>
       <c r="X52" s="2">
         <v>3035</v>
       </c>
-      <c r="Z52" s="10"/>
+      <c r="Z52" s="9"/>
       <c r="AA52" s="2">
         <v>4064</v>
       </c>
@@ -7470,14 +7645,14 @@
       <c r="T53" s="2">
         <v>1340</v>
       </c>
-      <c r="V53" s="10"/>
+      <c r="V53" s="9"/>
       <c r="W53" s="2">
         <v>1171</v>
       </c>
       <c r="X53" s="2">
         <v>3035</v>
       </c>
-      <c r="Z53" s="10"/>
+      <c r="Z53" s="9"/>
       <c r="AA53" s="2">
         <v>4054</v>
       </c>
@@ -7522,21 +7697,21 @@
       <c r="P54" s="2">
         <v>396</v>
       </c>
-      <c r="R54" s="9"/>
+      <c r="R54" s="8"/>
       <c r="S54" s="3">
         <v>1734</v>
       </c>
       <c r="T54" s="2">
         <v>1327</v>
       </c>
-      <c r="V54" s="10"/>
+      <c r="V54" s="9"/>
       <c r="W54" s="2">
         <v>1197</v>
       </c>
       <c r="X54" s="2">
         <v>3038</v>
       </c>
-      <c r="Z54" s="10"/>
+      <c r="Z54" s="9"/>
       <c r="AA54" s="2">
         <v>4041</v>
       </c>
@@ -7581,21 +7756,21 @@
       <c r="P55" s="2">
         <v>395</v>
       </c>
-      <c r="R55" s="9"/>
+      <c r="R55" s="8"/>
       <c r="S55" s="2">
         <v>1720</v>
       </c>
       <c r="T55" s="2">
         <v>1336</v>
       </c>
-      <c r="V55" s="10"/>
+      <c r="V55" s="9"/>
       <c r="W55" s="2">
         <v>1271</v>
       </c>
       <c r="X55" s="2">
         <v>3029</v>
       </c>
-      <c r="Z55" s="10"/>
+      <c r="Z55" s="9"/>
       <c r="AA55" s="2">
         <v>4265</v>
       </c>
@@ -7640,21 +7815,21 @@
       <c r="P56" s="2">
         <v>395</v>
       </c>
-      <c r="R56" s="9"/>
+      <c r="R56" s="8"/>
       <c r="S56" s="2">
         <v>1724</v>
       </c>
       <c r="T56" s="2">
         <v>1336</v>
       </c>
-      <c r="V56" s="10"/>
+      <c r="V56" s="9"/>
       <c r="W56" s="2">
         <v>1292</v>
       </c>
       <c r="X56" s="2">
         <v>3029</v>
       </c>
-      <c r="Z56" s="10"/>
+      <c r="Z56" s="9"/>
       <c r="AA56" s="2">
         <v>4500</v>
       </c>
@@ -7699,21 +7874,21 @@
       <c r="P57" s="2">
         <v>395</v>
       </c>
-      <c r="R57" s="9"/>
+      <c r="R57" s="8"/>
       <c r="S57" s="2">
         <v>1714</v>
       </c>
       <c r="T57" s="2">
         <v>1335</v>
       </c>
-      <c r="V57" s="10"/>
+      <c r="V57" s="9"/>
       <c r="W57" s="2">
         <v>1322</v>
       </c>
       <c r="X57" s="2">
         <v>3041</v>
       </c>
-      <c r="Z57" s="10"/>
+      <c r="Z57" s="9"/>
       <c r="AA57" s="2">
         <v>4100</v>
       </c>
@@ -7758,21 +7933,21 @@
       <c r="P58" s="2">
         <v>395</v>
       </c>
-      <c r="R58" s="9"/>
+      <c r="R58" s="8"/>
       <c r="S58" s="2">
         <v>1715</v>
       </c>
       <c r="T58" s="2">
         <v>1335</v>
       </c>
-      <c r="V58" s="10"/>
+      <c r="V58" s="9"/>
       <c r="W58" s="2">
         <v>1276</v>
       </c>
       <c r="X58" s="2">
         <v>3036</v>
       </c>
-      <c r="Z58" s="10"/>
+      <c r="Z58" s="9"/>
       <c r="AA58" s="2">
         <v>4080</v>
       </c>
@@ -7817,21 +7992,21 @@
       <c r="P59" s="2">
         <v>393</v>
       </c>
-      <c r="R59" s="9"/>
+      <c r="R59" s="8"/>
       <c r="S59" s="2">
         <v>1719</v>
       </c>
       <c r="T59" s="2">
         <v>1334</v>
       </c>
-      <c r="V59" s="10"/>
+      <c r="V59" s="9"/>
       <c r="W59" s="2">
         <v>1178</v>
       </c>
       <c r="X59" s="2">
         <v>3032</v>
       </c>
-      <c r="Z59" s="10"/>
+      <c r="Z59" s="9"/>
       <c r="AA59" s="2">
         <v>4073</v>
       </c>
@@ -7876,21 +8051,21 @@
       <c r="P60" s="2">
         <v>394</v>
       </c>
-      <c r="R60" s="9"/>
+      <c r="R60" s="8"/>
       <c r="S60" s="2">
         <v>1725</v>
       </c>
       <c r="T60" s="2">
         <v>1340</v>
       </c>
-      <c r="V60" s="10"/>
+      <c r="V60" s="9"/>
       <c r="W60" s="2">
         <v>1182</v>
       </c>
       <c r="X60" s="2">
         <v>3036</v>
       </c>
-      <c r="Z60" s="10"/>
+      <c r="Z60" s="9"/>
       <c r="AA60" s="2">
         <v>4059</v>
       </c>
@@ -7935,21 +8110,21 @@
       <c r="P61" s="2">
         <v>396</v>
       </c>
-      <c r="R61" s="9"/>
+      <c r="R61" s="8"/>
       <c r="S61" s="2">
         <v>1731</v>
       </c>
       <c r="T61" s="2">
         <v>1331</v>
       </c>
-      <c r="V61" s="10"/>
+      <c r="V61" s="9"/>
       <c r="W61" s="2">
         <v>1178</v>
       </c>
       <c r="X61" s="2">
         <v>3040</v>
       </c>
-      <c r="Z61" s="10"/>
+      <c r="Z61" s="9"/>
       <c r="AA61" s="2">
         <v>4052</v>
       </c>
@@ -7994,21 +8169,21 @@
       <c r="P62" s="2">
         <v>395</v>
       </c>
-      <c r="R62" s="9"/>
+      <c r="R62" s="8"/>
       <c r="S62" s="2">
         <v>1735</v>
       </c>
       <c r="T62" s="2">
         <v>1338</v>
       </c>
-      <c r="V62" s="10"/>
+      <c r="V62" s="9"/>
       <c r="W62" s="2">
         <v>1169</v>
       </c>
       <c r="X62" s="2">
         <v>3036</v>
       </c>
-      <c r="Z62" s="10"/>
+      <c r="Z62" s="9"/>
       <c r="AA62" s="2">
         <v>4071</v>
       </c>
@@ -8053,21 +8228,21 @@
       <c r="P63" s="2">
         <v>393</v>
       </c>
-      <c r="R63" s="9"/>
+      <c r="R63" s="8"/>
       <c r="S63" s="2">
         <v>1732</v>
       </c>
       <c r="T63" s="2">
         <v>1333</v>
       </c>
-      <c r="V63" s="10"/>
+      <c r="V63" s="9"/>
       <c r="W63" s="2">
         <v>1165</v>
       </c>
       <c r="X63" s="2">
         <v>3041</v>
       </c>
-      <c r="Z63" s="10"/>
+      <c r="Z63" s="9"/>
       <c r="AA63" s="2">
         <v>4538</v>
       </c>
@@ -8112,21 +8287,21 @@
       <c r="P64" s="2">
         <v>396</v>
       </c>
-      <c r="R64" s="9"/>
+      <c r="R64" s="8"/>
       <c r="S64" s="2">
         <v>1730</v>
       </c>
       <c r="T64" s="2">
         <v>1335</v>
       </c>
-      <c r="V64" s="10"/>
+      <c r="V64" s="9"/>
       <c r="W64" s="2">
         <v>1157</v>
       </c>
       <c r="X64" s="2">
         <v>3031</v>
       </c>
-      <c r="Z64" s="10"/>
+      <c r="Z64" s="9"/>
       <c r="AA64" s="2">
         <v>4143</v>
       </c>
@@ -8171,21 +8346,21 @@
       <c r="P65" s="2">
         <v>394</v>
       </c>
-      <c r="R65" s="9"/>
+      <c r="R65" s="8"/>
       <c r="S65" s="2">
         <v>1727</v>
       </c>
       <c r="T65" s="2">
         <v>1334</v>
       </c>
-      <c r="V65" s="10"/>
+      <c r="V65" s="9"/>
       <c r="W65" s="2">
         <v>1164</v>
       </c>
       <c r="X65" s="2">
         <v>3030</v>
       </c>
-      <c r="Z65" s="10"/>
+      <c r="Z65" s="9"/>
       <c r="AA65" s="2">
         <v>4078</v>
       </c>
@@ -8230,21 +8405,21 @@
       <c r="P66" s="2">
         <v>394</v>
       </c>
-      <c r="R66" s="9"/>
+      <c r="R66" s="8"/>
       <c r="S66" s="2">
         <v>1720</v>
       </c>
       <c r="T66" s="2">
         <v>1336</v>
       </c>
-      <c r="V66" s="10"/>
+      <c r="V66" s="9"/>
       <c r="W66" s="2">
         <v>1160</v>
       </c>
       <c r="X66" s="2">
         <v>3041</v>
       </c>
-      <c r="Z66" s="10"/>
+      <c r="Z66" s="9"/>
       <c r="AA66" s="2">
         <v>4072</v>
       </c>
@@ -8289,21 +8464,21 @@
       <c r="P67" s="2">
         <v>395</v>
       </c>
-      <c r="R67" s="9"/>
+      <c r="R67" s="8"/>
       <c r="S67" s="2">
         <v>1716</v>
       </c>
       <c r="T67" s="2">
         <v>1339</v>
       </c>
-      <c r="V67" s="10"/>
+      <c r="V67" s="9"/>
       <c r="W67" s="2">
         <v>1158</v>
       </c>
       <c r="X67" s="2">
         <v>3037</v>
       </c>
-      <c r="Z67" s="10"/>
+      <c r="Z67" s="9"/>
       <c r="AA67" s="2">
         <v>4038</v>
       </c>
@@ -8348,21 +8523,21 @@
       <c r="P68" s="2">
         <v>394</v>
       </c>
-      <c r="R68" s="9"/>
+      <c r="R68" s="8"/>
       <c r="S68" s="2">
         <v>1727</v>
       </c>
       <c r="T68" s="2">
         <v>1334</v>
       </c>
-      <c r="V68" s="10"/>
+      <c r="V68" s="9"/>
       <c r="W68" s="2">
         <v>1155</v>
       </c>
       <c r="X68" s="2">
         <v>3035</v>
       </c>
-      <c r="Z68" s="10"/>
+      <c r="Z68" s="9"/>
       <c r="AA68" s="2">
         <v>4054</v>
       </c>
@@ -8407,21 +8582,21 @@
       <c r="P69" s="2">
         <v>398</v>
       </c>
-      <c r="R69" s="9"/>
+      <c r="R69" s="8"/>
       <c r="S69" s="2">
         <v>1727</v>
       </c>
       <c r="T69" s="2">
         <v>1336</v>
       </c>
-      <c r="V69" s="10"/>
+      <c r="V69" s="9"/>
       <c r="W69" s="2">
         <v>1153</v>
       </c>
       <c r="X69" s="2">
         <v>3034</v>
       </c>
-      <c r="Z69" s="10"/>
+      <c r="Z69" s="9"/>
       <c r="AA69" s="2">
         <v>4055</v>
       </c>
@@ -8466,21 +8641,21 @@
       <c r="P70" s="2">
         <v>395</v>
       </c>
-      <c r="R70" s="9"/>
+      <c r="R70" s="8"/>
       <c r="S70" s="2">
         <v>1745</v>
       </c>
       <c r="T70" s="2">
         <v>1337</v>
       </c>
-      <c r="V70" s="10"/>
+      <c r="V70" s="9"/>
       <c r="W70" s="2">
         <v>1149</v>
       </c>
       <c r="X70" s="2">
         <v>3021</v>
       </c>
-      <c r="Z70" s="10"/>
+      <c r="Z70" s="9"/>
       <c r="AA70" s="2">
         <v>4279</v>
       </c>
@@ -8525,21 +8700,21 @@
       <c r="P71" s="2">
         <v>394</v>
       </c>
-      <c r="R71" s="9"/>
+      <c r="R71" s="8"/>
       <c r="S71" s="2">
         <v>1730</v>
       </c>
       <c r="T71" s="2">
         <v>1334</v>
       </c>
-      <c r="V71" s="10"/>
+      <c r="V71" s="9"/>
       <c r="W71" s="2">
         <v>1156</v>
       </c>
       <c r="X71" s="2">
         <v>3042</v>
       </c>
-      <c r="Z71" s="10"/>
+      <c r="Z71" s="9"/>
       <c r="AA71" s="2">
         <v>4487</v>
       </c>
@@ -8584,21 +8759,21 @@
       <c r="P72" s="2">
         <v>293</v>
       </c>
-      <c r="R72" s="9"/>
+      <c r="R72" s="8"/>
       <c r="S72" s="2">
         <v>1734</v>
       </c>
       <c r="T72" s="2">
         <v>1338</v>
       </c>
-      <c r="V72" s="10"/>
+      <c r="V72" s="9"/>
       <c r="W72" s="2">
         <v>1158</v>
       </c>
       <c r="X72" s="2">
         <v>3035</v>
       </c>
-      <c r="Z72" s="10"/>
+      <c r="Z72" s="9"/>
       <c r="AA72" s="2">
         <v>4118</v>
       </c>
@@ -8643,21 +8818,21 @@
       <c r="P73" s="2">
         <v>293</v>
       </c>
-      <c r="R73" s="9"/>
+      <c r="R73" s="8"/>
       <c r="S73" s="2">
         <v>1720</v>
       </c>
       <c r="T73" s="2">
         <v>1335</v>
       </c>
-      <c r="V73" s="10"/>
+      <c r="V73" s="9"/>
       <c r="W73" s="2">
         <v>1164</v>
       </c>
       <c r="X73" s="2">
         <v>3028</v>
       </c>
-      <c r="Z73" s="10"/>
+      <c r="Z73" s="9"/>
       <c r="AA73" s="2">
         <v>4106</v>
       </c>
@@ -8702,21 +8877,21 @@
       <c r="P74" s="2">
         <v>394</v>
       </c>
-      <c r="R74" s="9"/>
+      <c r="R74" s="8"/>
       <c r="S74" s="2">
         <v>1729</v>
       </c>
       <c r="T74" s="2">
         <v>1336</v>
       </c>
-      <c r="V74" s="10"/>
+      <c r="V74" s="9"/>
       <c r="W74" s="2">
         <v>1155</v>
       </c>
       <c r="X74" s="2">
         <v>3036</v>
       </c>
-      <c r="Z74" s="10"/>
+      <c r="Z74" s="9"/>
       <c r="AA74" s="2">
         <v>4074</v>
       </c>
@@ -8761,21 +8936,21 @@
       <c r="P75" s="2">
         <v>395</v>
       </c>
-      <c r="R75" s="9"/>
+      <c r="R75" s="8"/>
       <c r="S75" s="2">
         <v>1728</v>
       </c>
       <c r="T75" s="2">
         <v>1336</v>
       </c>
-      <c r="V75" s="10"/>
+      <c r="V75" s="9"/>
       <c r="W75" s="2">
         <v>1158</v>
       </c>
       <c r="X75" s="2">
         <v>3052</v>
       </c>
-      <c r="Z75" s="10"/>
+      <c r="Z75" s="9"/>
       <c r="AA75" s="2">
         <v>4087</v>
       </c>
@@ -8820,21 +8995,21 @@
       <c r="P76" s="2">
         <v>394</v>
       </c>
-      <c r="R76" s="9"/>
+      <c r="R76" s="8"/>
       <c r="S76" s="2">
         <v>1724</v>
       </c>
       <c r="T76" s="2">
         <v>1336</v>
       </c>
-      <c r="V76" s="10"/>
+      <c r="V76" s="9"/>
       <c r="W76" s="2">
         <v>1156</v>
       </c>
       <c r="X76" s="2">
         <v>3044</v>
       </c>
-      <c r="Z76" s="10"/>
+      <c r="Z76" s="9"/>
       <c r="AA76" s="2">
         <v>4067</v>
       </c>
@@ -8879,21 +9054,21 @@
       <c r="P77" s="2">
         <v>400</v>
       </c>
-      <c r="R77" s="9"/>
+      <c r="R77" s="8"/>
       <c r="S77" s="2">
         <v>1727</v>
       </c>
       <c r="T77" s="2">
         <v>1338</v>
       </c>
-      <c r="V77" s="10"/>
+      <c r="V77" s="9"/>
       <c r="W77" s="2">
         <v>1152</v>
       </c>
       <c r="X77" s="2">
         <v>3052</v>
       </c>
-      <c r="Z77" s="10"/>
+      <c r="Z77" s="9"/>
       <c r="AA77" s="2">
         <v>4089</v>
       </c>
@@ -8938,21 +9113,21 @@
       <c r="P78" s="2">
         <v>394</v>
       </c>
-      <c r="R78" s="9"/>
+      <c r="R78" s="8"/>
       <c r="S78" s="2">
         <v>1720</v>
       </c>
       <c r="T78" s="2">
         <v>1334</v>
       </c>
-      <c r="V78" s="10"/>
+      <c r="V78" s="9"/>
       <c r="W78" s="2">
         <v>1163</v>
       </c>
       <c r="X78" s="2">
         <v>3037</v>
       </c>
-      <c r="Z78" s="10"/>
+      <c r="Z78" s="9"/>
       <c r="AA78" s="2">
         <v>4521</v>
       </c>
@@ -8997,21 +9172,21 @@
       <c r="P79" s="2">
         <v>394</v>
       </c>
-      <c r="R79" s="9"/>
+      <c r="R79" s="8"/>
       <c r="S79" s="2">
         <v>1714</v>
       </c>
       <c r="T79" s="2">
         <v>1335</v>
       </c>
-      <c r="V79" s="10"/>
+      <c r="V79" s="9"/>
       <c r="W79" s="2">
         <v>1163</v>
       </c>
       <c r="X79" s="2">
         <v>3038</v>
       </c>
-      <c r="Z79" s="10"/>
+      <c r="Z79" s="9"/>
       <c r="AA79" s="2">
         <v>4111</v>
       </c>
@@ -9056,21 +9231,21 @@
       <c r="P80" s="2">
         <v>395</v>
       </c>
-      <c r="R80" s="9"/>
+      <c r="R80" s="8"/>
       <c r="S80" s="2">
         <v>1725</v>
       </c>
       <c r="T80" s="2">
         <v>1338</v>
       </c>
-      <c r="V80" s="10"/>
+      <c r="V80" s="9"/>
       <c r="W80" s="2">
         <v>1226</v>
       </c>
       <c r="X80" s="2">
         <v>3039</v>
       </c>
-      <c r="Z80" s="10"/>
+      <c r="Z80" s="9"/>
       <c r="AA80" s="2">
         <v>4094</v>
       </c>
@@ -9115,21 +9290,21 @@
       <c r="P81" s="2">
         <v>395</v>
       </c>
-      <c r="R81" s="9"/>
+      <c r="R81" s="8"/>
       <c r="S81" s="2">
         <v>1723</v>
       </c>
       <c r="T81" s="2">
         <v>1338</v>
       </c>
-      <c r="V81" s="10"/>
+      <c r="V81" s="9"/>
       <c r="W81" s="2">
         <v>1273</v>
       </c>
       <c r="X81" s="2">
         <v>3033</v>
       </c>
-      <c r="Z81" s="10"/>
+      <c r="Z81" s="9"/>
       <c r="AA81" s="2">
         <v>4068</v>
       </c>
@@ -9174,21 +9349,21 @@
       <c r="P82" s="2">
         <v>394</v>
       </c>
-      <c r="R82" s="9"/>
+      <c r="R82" s="8"/>
       <c r="S82" s="2">
         <v>1727</v>
       </c>
       <c r="T82" s="2">
         <v>1333</v>
       </c>
-      <c r="V82" s="10"/>
+      <c r="V82" s="9"/>
       <c r="W82" s="2">
         <v>1278</v>
       </c>
       <c r="X82" s="2">
         <v>3041</v>
       </c>
-      <c r="Z82" s="10"/>
+      <c r="Z82" s="9"/>
       <c r="AA82" s="2">
         <v>4069</v>
       </c>
@@ -9233,21 +9408,21 @@
       <c r="P83" s="2">
         <v>393</v>
       </c>
-      <c r="R83" s="9"/>
+      <c r="R83" s="8"/>
       <c r="S83" s="2">
         <v>1733</v>
       </c>
       <c r="T83" s="2">
         <v>1339</v>
       </c>
-      <c r="V83" s="10"/>
+      <c r="V83" s="9"/>
       <c r="W83" s="2">
         <v>1314</v>
       </c>
       <c r="X83" s="2">
         <v>3046</v>
       </c>
-      <c r="Z83" s="10"/>
+      <c r="Z83" s="9"/>
       <c r="AA83" s="2">
         <v>4084</v>
       </c>
@@ -9292,21 +9467,21 @@
       <c r="P84" s="2">
         <v>400</v>
       </c>
-      <c r="R84" s="9"/>
+      <c r="R84" s="8"/>
       <c r="S84" s="2">
         <v>1727</v>
       </c>
       <c r="T84" s="2">
         <v>1336</v>
       </c>
-      <c r="V84" s="10"/>
+      <c r="V84" s="9"/>
       <c r="W84" s="2">
         <v>1284</v>
       </c>
       <c r="X84" s="2">
         <v>3033</v>
       </c>
-      <c r="Z84" s="10"/>
+      <c r="Z84" s="9"/>
       <c r="AA84" s="2">
         <v>4043</v>
       </c>
@@ -9351,21 +9526,21 @@
       <c r="P85" s="2">
         <v>395</v>
       </c>
-      <c r="R85" s="9"/>
+      <c r="R85" s="8"/>
       <c r="S85" s="2">
         <v>1729</v>
       </c>
       <c r="T85" s="2">
         <v>1333</v>
       </c>
-      <c r="V85" s="10"/>
+      <c r="V85" s="9"/>
       <c r="W85" s="2">
         <v>1199</v>
       </c>
       <c r="X85" s="2">
         <v>3043</v>
       </c>
-      <c r="Z85" s="10"/>
+      <c r="Z85" s="9"/>
       <c r="AA85" s="2">
         <v>4270</v>
       </c>
@@ -9410,21 +9585,21 @@
       <c r="P86" s="2">
         <v>394</v>
       </c>
-      <c r="R86" s="9"/>
+      <c r="R86" s="8"/>
       <c r="S86" s="2">
         <v>1721</v>
       </c>
       <c r="T86" s="2">
         <v>1336</v>
       </c>
-      <c r="V86" s="10"/>
+      <c r="V86" s="9"/>
       <c r="W86" s="2">
         <v>1188</v>
       </c>
       <c r="X86" s="2">
         <v>3035</v>
       </c>
-      <c r="Z86" s="10"/>
+      <c r="Z86" s="9"/>
       <c r="AA86" s="2">
         <v>4259</v>
       </c>
@@ -9469,21 +9644,21 @@
       <c r="P87" s="2">
         <v>395</v>
       </c>
-      <c r="R87" s="9"/>
+      <c r="R87" s="8"/>
       <c r="S87" s="2">
         <v>1716</v>
       </c>
       <c r="T87" s="2">
         <v>1334</v>
       </c>
-      <c r="V87" s="10"/>
+      <c r="V87" s="9"/>
       <c r="W87" s="2">
         <v>1174</v>
       </c>
       <c r="X87" s="2">
         <v>3042</v>
       </c>
-      <c r="Z87" s="10"/>
+      <c r="Z87" s="9"/>
       <c r="AA87" s="2">
         <v>4080</v>
       </c>
@@ -9528,21 +9703,21 @@
       <c r="P88" s="2">
         <v>394</v>
       </c>
-      <c r="R88" s="9"/>
+      <c r="R88" s="8"/>
       <c r="S88" s="2">
         <v>1728</v>
       </c>
       <c r="T88" s="2">
         <v>1338</v>
       </c>
-      <c r="V88" s="10"/>
+      <c r="V88" s="9"/>
       <c r="W88" s="2">
         <v>1173</v>
       </c>
       <c r="X88" s="2">
         <v>3029</v>
       </c>
-      <c r="Z88" s="10"/>
+      <c r="Z88" s="9"/>
       <c r="AA88" s="2">
         <v>4077</v>
       </c>
@@ -9587,21 +9762,21 @@
       <c r="P89" s="2">
         <v>294</v>
       </c>
-      <c r="R89" s="9"/>
+      <c r="R89" s="8"/>
       <c r="S89" s="2">
         <v>1722</v>
       </c>
       <c r="T89" s="2">
         <v>1336</v>
       </c>
-      <c r="V89" s="10"/>
+      <c r="V89" s="9"/>
       <c r="W89" s="2">
         <v>1175</v>
       </c>
       <c r="X89" s="2">
         <v>3038</v>
       </c>
-      <c r="Z89" s="10"/>
+      <c r="Z89" s="9"/>
       <c r="AA89" s="2">
         <v>4073</v>
       </c>
@@ -9646,21 +9821,21 @@
       <c r="P90" s="2">
         <v>296</v>
       </c>
-      <c r="R90" s="9"/>
+      <c r="R90" s="8"/>
       <c r="S90" s="2">
         <v>1724</v>
       </c>
       <c r="T90" s="2">
         <v>1340</v>
       </c>
-      <c r="V90" s="10"/>
+      <c r="V90" s="9"/>
       <c r="W90" s="2">
         <v>1171</v>
       </c>
       <c r="X90" s="2">
         <v>3049</v>
       </c>
-      <c r="Z90" s="10"/>
+      <c r="Z90" s="9"/>
       <c r="AA90" s="2">
         <v>4073</v>
       </c>
@@ -9705,21 +9880,21 @@
       <c r="P91" s="2">
         <v>388</v>
       </c>
-      <c r="R91" s="9"/>
+      <c r="R91" s="8"/>
       <c r="S91" s="2">
         <v>1733</v>
       </c>
       <c r="T91" s="2">
         <v>1338</v>
       </c>
-      <c r="V91" s="10"/>
+      <c r="V91" s="9"/>
       <c r="W91" s="2">
         <v>1164</v>
       </c>
       <c r="X91" s="2">
         <v>3033</v>
       </c>
-      <c r="Z91" s="10"/>
+      <c r="Z91" s="9"/>
       <c r="AA91" s="2">
         <v>4062</v>
       </c>
@@ -9764,21 +9939,21 @@
       <c r="P92" s="2">
         <v>400</v>
       </c>
-      <c r="R92" s="9"/>
+      <c r="R92" s="8"/>
       <c r="S92" s="2">
         <v>1716</v>
       </c>
       <c r="T92" s="2">
         <v>1337</v>
       </c>
-      <c r="V92" s="10"/>
+      <c r="V92" s="9"/>
       <c r="W92" s="2">
         <v>1170</v>
       </c>
       <c r="X92" s="2">
         <v>3033</v>
       </c>
-      <c r="Z92" s="10"/>
+      <c r="Z92" s="9"/>
       <c r="AA92" s="2">
         <v>4081</v>
       </c>
@@ -9823,21 +9998,21 @@
       <c r="P93" s="2">
         <v>251</v>
       </c>
-      <c r="R93" s="9"/>
+      <c r="R93" s="8"/>
       <c r="S93" s="2">
         <v>1722</v>
       </c>
       <c r="T93" s="2">
         <v>1337</v>
       </c>
-      <c r="V93" s="10"/>
+      <c r="V93" s="9"/>
       <c r="W93" s="2">
         <v>1158</v>
       </c>
       <c r="X93" s="2">
         <v>3032</v>
       </c>
-      <c r="Z93" s="10"/>
+      <c r="Z93" s="9"/>
       <c r="AA93" s="2">
         <v>4084</v>
       </c>
@@ -9882,21 +10057,21 @@
       <c r="P94" s="2">
         <v>234</v>
       </c>
-      <c r="R94" s="9"/>
+      <c r="R94" s="8"/>
       <c r="S94" s="2">
         <v>1723</v>
       </c>
       <c r="T94" s="2">
         <v>1336</v>
       </c>
-      <c r="V94" s="10"/>
+      <c r="V94" s="9"/>
       <c r="W94" s="2">
         <v>1164</v>
       </c>
       <c r="X94" s="2">
         <v>3036</v>
       </c>
-      <c r="Z94" s="10"/>
+      <c r="Z94" s="9"/>
       <c r="AA94" s="2">
         <v>4118</v>
       </c>
@@ -9941,21 +10116,21 @@
       <c r="P95" s="2">
         <v>235</v>
       </c>
-      <c r="R95" s="9"/>
+      <c r="R95" s="8"/>
       <c r="S95" s="2">
         <v>1730</v>
       </c>
       <c r="T95" s="2">
         <v>1332</v>
       </c>
-      <c r="V95" s="10"/>
+      <c r="V95" s="9"/>
       <c r="W95" s="2">
         <v>1169</v>
       </c>
       <c r="X95" s="2">
         <v>3033</v>
       </c>
-      <c r="Z95" s="10"/>
+      <c r="Z95" s="9"/>
       <c r="AA95" s="2">
         <v>4118</v>
       </c>
@@ -10000,21 +10175,21 @@
       <c r="P96" s="2">
         <v>235</v>
       </c>
-      <c r="R96" s="9"/>
+      <c r="R96" s="8"/>
       <c r="S96" s="2">
         <v>1720</v>
       </c>
       <c r="T96" s="2">
         <v>1337</v>
       </c>
-      <c r="V96" s="10"/>
+      <c r="V96" s="9"/>
       <c r="W96" s="2">
         <v>1174</v>
       </c>
       <c r="X96" s="2">
         <v>3041</v>
       </c>
-      <c r="Z96" s="10"/>
+      <c r="Z96" s="9"/>
       <c r="AA96" s="2">
         <v>4062</v>
       </c>
@@ -10059,21 +10234,21 @@
       <c r="P97" s="2">
         <v>234</v>
       </c>
-      <c r="R97" s="9"/>
+      <c r="R97" s="8"/>
       <c r="S97" s="2">
         <v>1724</v>
       </c>
       <c r="T97" s="2">
         <v>1341</v>
       </c>
-      <c r="V97" s="10"/>
+      <c r="V97" s="9"/>
       <c r="W97" s="2">
         <v>1164</v>
       </c>
       <c r="X97" s="2">
         <v>3029</v>
       </c>
-      <c r="Z97" s="10"/>
+      <c r="Z97" s="9"/>
       <c r="AA97" s="2">
         <v>4089</v>
       </c>
@@ -10118,21 +10293,21 @@
       <c r="P98" s="2">
         <v>235</v>
       </c>
-      <c r="R98" s="9"/>
+      <c r="R98" s="8"/>
       <c r="S98" s="2">
         <v>1714</v>
       </c>
       <c r="T98" s="2">
         <v>1338</v>
       </c>
-      <c r="V98" s="10"/>
+      <c r="V98" s="9"/>
       <c r="W98" s="2">
         <v>1158</v>
       </c>
       <c r="X98" s="2">
         <v>3044</v>
       </c>
-      <c r="Z98" s="10"/>
+      <c r="Z98" s="9"/>
       <c r="AA98" s="2">
         <v>4089</v>
       </c>
@@ -10177,21 +10352,21 @@
       <c r="P99" s="2">
         <v>235</v>
       </c>
-      <c r="R99" s="9"/>
+      <c r="R99" s="8"/>
       <c r="S99" s="2">
         <v>1717</v>
       </c>
       <c r="T99" s="2">
         <v>1339</v>
       </c>
-      <c r="V99" s="10"/>
+      <c r="V99" s="9"/>
       <c r="W99" s="2">
         <v>1150</v>
       </c>
       <c r="X99" s="2">
         <v>3035</v>
       </c>
-      <c r="Z99" s="10"/>
+      <c r="Z99" s="9"/>
       <c r="AA99" s="2">
         <v>4093</v>
       </c>
@@ -10236,21 +10411,21 @@
       <c r="P100" s="2">
         <v>235</v>
       </c>
-      <c r="R100" s="9"/>
+      <c r="R100" s="8"/>
       <c r="S100" s="2">
         <v>1729</v>
       </c>
       <c r="T100" s="2">
         <v>1335</v>
       </c>
-      <c r="V100" s="10"/>
+      <c r="V100" s="9"/>
       <c r="W100" s="2">
         <v>1153</v>
       </c>
       <c r="X100" s="2">
         <v>3040</v>
       </c>
-      <c r="Z100" s="10"/>
+      <c r="Z100" s="9"/>
       <c r="AA100" s="2">
         <v>4182</v>
       </c>
@@ -10295,21 +10470,21 @@
       <c r="P101" s="2">
         <v>234</v>
       </c>
-      <c r="R101" s="9"/>
+      <c r="R101" s="8"/>
       <c r="S101" s="2">
         <v>1719</v>
       </c>
       <c r="T101" s="2">
         <v>1335</v>
       </c>
-      <c r="V101" s="10"/>
+      <c r="V101" s="9"/>
       <c r="W101" s="2">
         <v>1152</v>
       </c>
       <c r="X101" s="2">
         <v>3039</v>
       </c>
-      <c r="Z101" s="10"/>
+      <c r="Z101" s="9"/>
       <c r="AA101" s="2">
         <v>4110</v>
       </c>
@@ -10354,21 +10529,21 @@
       <c r="P102" s="2">
         <v>234</v>
       </c>
-      <c r="R102" s="9"/>
+      <c r="R102" s="8"/>
       <c r="S102" s="2">
         <v>1719</v>
       </c>
       <c r="T102" s="2">
         <v>1335</v>
       </c>
-      <c r="V102" s="10"/>
+      <c r="V102" s="9"/>
       <c r="W102" s="2">
         <v>1156</v>
       </c>
       <c r="X102" s="2">
         <v>3036</v>
       </c>
-      <c r="Z102" s="10"/>
+      <c r="Z102" s="9"/>
       <c r="AA102" s="2">
         <v>4452</v>
       </c>
@@ -10413,21 +10588,21 @@
       <c r="P103" s="2">
         <v>235</v>
       </c>
-      <c r="R103" s="9"/>
+      <c r="R103" s="8"/>
       <c r="S103" s="2">
         <v>1720</v>
       </c>
       <c r="T103" s="2">
         <v>1336</v>
       </c>
-      <c r="V103" s="10"/>
+      <c r="V103" s="9"/>
       <c r="W103" s="2">
         <v>1166</v>
       </c>
       <c r="X103" s="2">
         <v>3044</v>
       </c>
-      <c r="Z103" s="10"/>
+      <c r="Z103" s="9"/>
       <c r="AA103" s="2">
         <v>4076</v>
       </c>
@@ -10436,41 +10611,41 @@
       </c>
     </row>
     <row r="104" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="F104" s="9" t="s">
+      <c r="C104" s="8"/>
+      <c r="D104" s="8"/>
+      <c r="F104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="J104" s="9" t="s">
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="J104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="N104" s="9" t="s">
+      <c r="K104" s="8"/>
+      <c r="L104" s="8"/>
+      <c r="N104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O104" s="9"/>
-      <c r="P104" s="9"/>
-      <c r="R104" s="9" t="s">
+      <c r="O104" s="8"/>
+      <c r="P104" s="8"/>
+      <c r="R104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="S104" s="9"/>
-      <c r="T104" s="9"/>
-      <c r="V104" s="9" t="s">
+      <c r="S104" s="8"/>
+      <c r="T104" s="8"/>
+      <c r="V104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="W104" s="9"/>
-      <c r="X104" s="9"/>
-      <c r="Z104" s="9" t="s">
+      <c r="W104" s="8"/>
+      <c r="X104" s="8"/>
+      <c r="Z104" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AA104" s="9"/>
-      <c r="AB104" s="9"/>
+      <c r="AA104" s="8"/>
+      <c r="AB104" s="8"/>
     </row>
     <row r="105" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B105" s="2">
@@ -10566,8 +10741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9980FA75-0FD8-A448-82AA-5AA0CC5094F6}">
   <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10580,94 +10755,94 @@
   <sheetData>
     <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>6</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>8</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>9</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>10</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>12</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>13</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>118</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>1641</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>11371</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>102757</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>12171000</v>
       </c>
-      <c r="H3" s="14" t="str">
+      <c r="H3" s="13" t="str">
         <f>'Dane poszczególne'!V105</f>
         <v>N/A</v>
       </c>
-      <c r="I3" s="15" t="str">
+      <c r="I3" s="14" t="str">
         <f>'Dane poszczególne'!Z105</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>181</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>1113</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>3642</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>4261</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>77462</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>109396</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="17">
         <v>407387</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>

</xml_diff>